<commit_message>
Adding code to grab information out the database for the favorites sections
</commit_message>
<xml_diff>
--- a/assets/Lego Descriptions.xlsx
+++ b/assets/Lego Descriptions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal Files\Janets Work\House of Legos\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janet\Documents\My Web Sites\House-of-Legos-Yoder\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>Millenium Falcon</t>
   </si>
@@ -189,12 +189,21 @@
   <si>
     <t>Command the Clone Army against the Separatists with buildable Obi-Wan Kenobi. With durable, fully posable limbs, special white Clone armor, fabric cape, buildable blue Lightsaber and a holster with extra Lightsaber handle, this LEGO® Jedi Master is ready for tough action play!</t>
   </si>
+  <si>
+    <t xml:space="preserve">LEGO Harry Potter Hogwart's Express </t>
+  </si>
+  <si>
+    <t>Includes 5 minifigures: Harry Potter, Ron Weasley, Ginny Weasley, Luna Lovegood and Draco Malfoy
+Hogwarts Express accessories include food trolley, suitcases, ice cream, owls, Invisibility Cloak and more
+Remove passenger car roof to reveal inside
+Open baggage compartment</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,6 +240,27 @@
       <color rgb="FF3B3B3B"/>
       <name val="Inherit"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF111111"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF111111"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF111111"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -252,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -267,6 +297,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -732,6 +771,32 @@
         <v>27</v>
       </c>
     </row>
+    <row r="12" spans="1:5" ht="86.4">
+      <c r="A12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12">
+        <v>4841</v>
+      </c>
+      <c r="C12">
+        <v>646</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="D13" s="10"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="D15" s="9"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>